<commit_message>
change the htm type of test output in txt, use uncompress tag in test and generate a new test file test.xls
</commit_message>
<xml_diff>
--- a/tools/facturation_ibps/test-data/test.xlsx
+++ b/tools/facturation_ibps/test-data/test.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="24300" windowWidth="34605" xWindow="14265" yWindow="4755"/>
   </bookViews>
   <sheets>
-    <sheet name="SMP-2011" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SMP-2011" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="152511" concurrentCalc="0" fullCalcOnLoad="1"/>
@@ -19,7 +19,7 @@
     <t>Relevé de prestation de service - A REGLER</t>
   </si>
   <si>
-    <t>imagerie-2018/ 217</t>
+    <t xml:space="preserve">  imagerie-2018/ 217</t>
   </si>
   <si>
     <t>référence à rappeler sur votre bon de commande</t>
@@ -127,7 +127,7 @@
     <t>77.00</t>
   </si>
   <si>
-    <t>21.00</t>
+    <t xml:space="preserve">21.00 </t>
   </si>
   <si>
     <t>Confocal SP5 Inversé 8-2018</t>
@@ -840,7 +840,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -855,13 +855,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1216,7 +1216,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1690,6 +1690,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>